<commit_message>
API over 50% complete
</commit_message>
<xml_diff>
--- a/hobi api docs.xlsx
+++ b/hobi api docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AE985B-403C-4006-950C-0CF4BB2E8CCE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A49E496-E9E3-42E3-BCB9-950A5080EE05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0F4B7B1A-6694-4032-A35B-9BC2F00461DD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
   <si>
     <t>STORED PROCEDURES</t>
   </si>
@@ -144,12 +144,6 @@
     <t>add mod privileges</t>
   </si>
   <si>
-    <t>(mod) accept member</t>
-  </si>
-  <si>
-    <t>(mod) decline member</t>
-  </si>
-  <si>
     <t>(mod) kick member</t>
   </si>
   <si>
@@ -180,7 +174,25 @@
     <t>edit user password</t>
   </si>
   <si>
-    <t>23% COMPLETE</t>
+    <t>(mod) accept member - Private group</t>
+  </si>
+  <si>
+    <t>(mod) decline member - private group</t>
+  </si>
+  <si>
+    <t>get group moderators</t>
+  </si>
+  <si>
+    <t>&gt; Needs testing</t>
+  </si>
+  <si>
+    <t>set group admin</t>
+  </si>
+  <si>
+    <t>(admin) add group moderator</t>
+  </si>
+  <si>
+    <t>(admin) Remove group moderator</t>
   </si>
 </sst>
 </file>
@@ -727,18 +739,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8D0841-E701-441C-B983-07B370312B6E}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.41796875" customWidth="1"/>
+    <col min="1" max="1" width="31.5234375" customWidth="1"/>
     <col min="2" max="2" width="18.05078125" customWidth="1"/>
     <col min="3" max="3" width="13.26171875" customWidth="1"/>
-    <col min="4" max="4" width="14.41796875" customWidth="1"/>
+    <col min="4" max="4" width="16.62890625" customWidth="1"/>
     <col min="5" max="5" width="23.578125" customWidth="1"/>
     <col min="6" max="6" width="24.26171875" customWidth="1"/>
   </cols>
@@ -765,8 +777,8 @@
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>14</v>
@@ -780,8 +792,8 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>4</v>
@@ -795,8 +807,11 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>15</v>
@@ -810,8 +825,8 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -821,8 +836,8 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -832,8 +847,8 @@
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>24</v>
@@ -850,8 +865,8 @@
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>6</v>
@@ -870,8 +885,8 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>25</v>
@@ -890,8 +905,8 @@
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="17"/>
@@ -906,8 +921,8 @@
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -920,8 +935,8 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="2"/>
@@ -936,14 +951,14 @@
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -956,8 +971,8 @@
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="2"/>
@@ -972,8 +987,8 @@
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="17"/>
@@ -988,8 +1003,8 @@
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="2"/>
@@ -1004,8 +1019,8 @@
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
+      <c r="C17" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="17"/>
@@ -1017,11 +1032,11 @@
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>15</v>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="2"/>
@@ -1033,11 +1048,11 @@
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="2"/>
@@ -1144,7 +1159,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>15</v>
@@ -1155,7 +1170,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>15</v>
@@ -1166,7 +1181,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>15</v>
@@ -1177,7 +1192,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>15</v>
@@ -1188,7 +1203,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>15</v>
@@ -1199,7 +1214,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>15</v>
@@ -1210,7 +1225,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>15</v>
@@ -1221,7 +1236,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>15</v>
@@ -1232,29 +1247,74 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="37" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="19">
-        <f>16/33 * 100</f>
-        <v>48.484848484848484</v>
-      </c>
-      <c r="C37" s="19">
-        <v>0</v>
-      </c>
-      <c r="D37" s="20" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
         <v>49</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="19">
+        <f>21/38 * 100</f>
+        <v>55.26315789473685</v>
+      </c>
+      <c r="C40" s="19">
+        <f>(21/38) * 100</f>
+        <v>55.26315789473685</v>
+      </c>
+      <c r="D40" s="20">
+        <f>(B40+C40)/2</f>
+        <v>55.26315789473685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>